<commit_message>
sudah masuk ke database
</commit_message>
<xml_diff>
--- a/data/data_hirarki2.xlsx
+++ b/data/data_hirarki2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Python\Riset\quran-tema\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BFE765-6920-42CA-AC17-CE635A6EA62F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C93EE8-1CB0-4512-AD5F-06600EC0BCA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="4155" windowWidth="17220" windowHeight="11295" xr2:uid="{CD02A47C-ECDF-4E8E-95B0-DE4F5A9BE3DA}"/>
+    <workbookView xWindow="7215" yWindow="1485" windowWidth="17220" windowHeight="11295" xr2:uid="{CD02A47C-ECDF-4E8E-95B0-DE4F5A9BE3DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Keutamaan ilmu</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Mmpi Yusuf as.</t>
-  </si>
-  <si>
-    <t>Level 5</t>
   </si>
   <si>
     <t>Qs.2:38</t>
@@ -559,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E453A-362A-4338-9914-9864CFE3FE9D}">
   <dimension ref="B3:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,16 +589,16 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -613,16 +610,16 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -643,16 +640,16 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -664,16 +661,16 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="I9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -756,27 +753,25 @@
         <v>17</v>
       </c>
       <c r="F18" s="1"/>
+      <c r="G18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
@@ -810,16 +805,16 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="J23" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mencoba cara baru untuk import data
</commit_message>
<xml_diff>
--- a/data/data_hirarki2.xlsx
+++ b/data/data_hirarki2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Python\Riset\quran-tema\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Python\Riset\Buk_Liza\try\boiler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C93EE8-1CB0-4512-AD5F-06600EC0BCA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF35EBB-AF99-4966-8F71-02B952CF6476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="1485" windowWidth="17220" windowHeight="11295" xr2:uid="{CD02A47C-ECDF-4E8E-95B0-DE4F5A9BE3DA}"/>
+    <workbookView xWindow="8520" yWindow="3075" windowWidth="14925" windowHeight="11325" xr2:uid="{CD02A47C-ECDF-4E8E-95B0-DE4F5A9BE3DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,19 +224,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{6EBBDC1B-C541-4BE0-A68B-FC4E62802862}"/>
@@ -554,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E453A-362A-4338-9914-9864CFE3FE9D}">
-  <dimension ref="B3:J34"/>
+  <dimension ref="B3:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,16 +604,16 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -639,16 +634,16 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -660,16 +655,16 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -753,69 +748,63 @@
         <v>17</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="F21" s="1"/>
+      <c r="G21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
@@ -833,22 +822,16 @@
       <c r="B28" s="1"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
+      <c r="B29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>